<commit_message>
Revert "Addition of clitics"
This reverts commit 29092932c8e9012eed054074f491688e4172bdb2.
</commit_message>
<xml_diff>
--- a/data/Trainingdata.xlsx
+++ b/data/Trainingdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kimbe\Documents\GitHub\read\read\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kimbe\Documents\GitHub\read\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -457,7 +457,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>